<commit_message>
Final list of CMIP6 models: temp, precip, snow and wind
</commit_message>
<xml_diff>
--- a/ATLAS-inventory/CMIP6/CMIP6_simulations_Atlas.xlsx
+++ b/ATLAS-inventory/CMIP6/CMIP6_simulations_Atlas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gutierjm/Desktop/tmp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05BD9384-85F9-AA4D-A855-FF523520C657}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{744C540B-B6EF-194C-8978-B912066ABE38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15500" yWindow="500" windowWidth="20000" windowHeight="19200" xr2:uid="{0263EA14-0FFA-D748-B725-70D994A0B932}"/>
+    <workbookView xWindow="9340" yWindow="460" windowWidth="25100" windowHeight="19920" xr2:uid="{0263EA14-0FFA-D748-B725-70D994A0B932}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="98">
   <si>
     <t>hist</t>
   </si>
@@ -95,9 +95,6 @@
     <t>Size</t>
   </si>
   <si>
-    <t>Size (GB) is the size of the dataset (only historical scenario)</t>
-  </si>
-  <si>
     <t>CMCC.CMCC-CM2-SR5</t>
   </si>
   <si>
@@ -209,19 +206,756 @@
     <t>SSP5.85</t>
   </si>
   <si>
-    <t>P T X</t>
-  </si>
-  <si>
-    <t>P T</t>
-  </si>
-  <si>
-    <t>T X</t>
-  </si>
-  <si>
     <t>The institution is "MPI-M." for this historical simulations  but "DKRZ." for the scenarios.</t>
   </si>
   <si>
-    <t>P: precipitation  T: mean temperature  X: Tmin and Tmax</t>
+    <t xml:space="preserve">MONTHLY - W: wind (sfcWind), S: snow (prsn) </t>
+  </si>
+  <si>
+    <t>CAS.FGOALS-f3-L</t>
+  </si>
+  <si>
+    <t>CCCma.CanESM5-CanOE</t>
+  </si>
+  <si>
+    <t>Suitable-BA</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>CMCC.CMCC-ESM2</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>P T X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>S W</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>T X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> S W</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t xml:space="preserve">P T </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>S W</t>
+    </r>
+  </si>
+  <si>
+    <t>EC-Earth-Consortium.EC-Earth3-CC</t>
+  </si>
+  <si>
+    <t>E3SM-Project.E3SM-1-1</t>
+  </si>
+  <si>
+    <t>S W</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">DAILY - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: precipitation (pr)  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">:  temperature (tas)  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: tasmin and tasmax</t>
+    </r>
+  </si>
+  <si>
+    <t>FIO-QLNM.FIO-ESM-2-0</t>
+  </si>
+  <si>
+    <t>IPSL.IPSL-CM5A2-INCA</t>
+  </si>
+  <si>
+    <t>MOHC.HadGEM3-GC31-MM</t>
+  </si>
+  <si>
+    <t>NASA-GISS.GISS-E2-1-G</t>
+  </si>
+  <si>
+    <t>Size (GB) is the size of the dataset (only historical scenario for the daily variables)</t>
+  </si>
+  <si>
+    <t>THU.CIESM</t>
+  </si>
+  <si>
+    <t>UA.MCM-UA-1-0</t>
+  </si>
+  <si>
+    <t>Models included in the ATLAS</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t xml:space="preserve">P T </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">S W </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>N</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>P T X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">S W </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">MONTHLY (land) - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: snow water equivalent (snw) and snow cover (snc). </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: total soil moisture (mrso) </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">S W </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">P T X </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t xml:space="preserve">S W </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>M</t>
+    </r>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t xml:space="preserve">TBC </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t xml:space="preserve">P T </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>S W</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t xml:space="preserve"> M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t xml:space="preserve">P T </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">W </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>P T X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">S W </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>TBC</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t xml:space="preserve"> M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t xml:space="preserve">X </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">S W </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t xml:space="preserve">T </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">S W </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">P T </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>S W</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t xml:space="preserve"> N</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t xml:space="preserve">P T </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">W </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">P T X </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>P T X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">S </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">S </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>M</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -231,7 +965,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -249,6 +983,54 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri (Cuerpo)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri (Cuerpo)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF24292E"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri (Cuerpo)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="5"/>
+      <name val="Calibri (Cuerpo)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Cuerpo)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="5"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -280,7 +1062,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -290,10 +1072,36 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -608,61 +1416,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07E30FBF-232B-8647-9316-8274C69113B8}">
-  <dimension ref="A1:L41"/>
+  <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="5.33203125" customWidth="1"/>
-    <col min="2" max="2" width="39.83203125" customWidth="1"/>
+    <col min="2" max="2" width="37.33203125" customWidth="1"/>
     <col min="3" max="3" width="9.33203125" customWidth="1"/>
     <col min="4" max="4" width="5.33203125" customWidth="1"/>
-    <col min="5" max="10" width="7.83203125" style="2" customWidth="1"/>
+    <col min="5" max="10" width="12.83203125" style="2" customWidth="1"/>
     <col min="11" max="11" width="7.5" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.1640625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:13" s="5" customFormat="1">
+      <c r="A1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13">
       <c r="A2">
         <v>1</v>
       </c>
@@ -676,19 +1488,31 @@
         <v>3</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="G2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>83</v>
+      </c>
       <c r="J2" s="4" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="K2" s="1">
         <v>80.864219671000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L2" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3">
         <v>2</v>
       </c>
@@ -702,28 +1526,31 @@
         <v>3</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="K3" s="1">
         <v>40.955032519</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L3" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4">
         <v>3</v>
       </c>
@@ -736,29 +1563,32 @@
       <c r="D4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>58</v>
+      <c r="E4" s="14" t="s">
+        <v>84</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>58</v>
+      <c r="G4" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>84</v>
       </c>
       <c r="K4" s="1">
         <v>61.678528151999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L4" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5">
         <v>4</v>
       </c>
@@ -772,28 +1602,28 @@
         <v>3</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>16</v>
+        <v>87</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>86</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
       <c r="K5" s="1">
         <v>49.374977031999997</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13">
       <c r="A6">
         <v>5</v>
       </c>
@@ -807,28 +1637,31 @@
         <v>3</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>16</v>
+        <v>81</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>86</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="K6" s="1">
         <v>17.579313868</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L6" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7">
         <v>6</v>
       </c>
@@ -842,28 +1675,31 @@
         <v>3</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="K7" s="1">
         <v>8.1137502799999996</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L7" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8">
         <v>7</v>
       </c>
@@ -877,33 +1713,33 @@
         <v>3</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="K8" s="1">
         <v>10.117401146000001</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
         <v>2</v>
@@ -912,33 +1748,36 @@
         <v>3</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="K9" s="1">
         <v>40.710173165999997</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L9" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
@@ -947,33 +1786,36 @@
         <v>6</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="K10" s="1">
         <v>172.948435115</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L10" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -982,33 +1824,36 @@
         <v>6</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="K11" s="1">
         <v>24.089237158</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L11" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -1017,33 +1862,36 @@
         <v>6</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="K12" s="1">
         <v>24.079629625999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L12" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
@@ -1052,33 +1900,36 @@
         <v>3</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="K13" s="1">
         <v>24.253234431999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L13" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
@@ -1087,33 +1938,36 @@
         <v>3</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="K14" s="1">
         <v>26.406662283999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L14" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
         <v>2</v>
@@ -1122,24 +1976,27 @@
         <v>6</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="K15" s="1">
         <v>115.687261263</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L15" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
@@ -1148,27 +2005,36 @@
         <v>6</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>16</v>
+        <v>90</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>81</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>81</v>
       </c>
       <c r="K16" s="1">
         <v>45.000454378999997</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L16" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
@@ -1177,33 +2043,36 @@
         <v>6</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="K17" s="1">
         <v>115.379159147</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L17" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
         <v>2</v>
@@ -1212,33 +2081,36 @@
         <v>6</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="K18" s="1">
         <v>115.73568678399999</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L18" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s">
         <v>2</v>
@@ -1247,24 +2119,27 @@
         <v>3</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="K19" s="1">
         <v>11.195230902</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L19" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
@@ -1273,33 +2148,36 @@
         <v>7</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="K20" s="1">
         <v>16.816434255000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L20" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
@@ -1308,33 +2186,36 @@
         <v>7</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="K21" s="1">
         <v>16.823844715</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L21" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C22" t="s">
         <v>2</v>
@@ -1343,33 +2224,36 @@
         <v>6</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="K22" s="1">
         <v>15.294436826</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L22" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C23" t="s">
         <v>2</v>
@@ -1378,30 +2262,33 @@
         <v>7</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="K23" s="1">
         <v>31.092069240000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L23" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24" t="s">
         <v>5</v>
@@ -1410,33 +2297,36 @@
         <v>3</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="K24" s="1">
         <v>6.1996430370000004</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L24" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C25" t="s">
         <v>2</v>
@@ -1445,33 +2335,36 @@
         <v>3</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="K25" s="1">
         <v>23.192044070000001</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L25" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C26" t="s">
         <v>8</v>
@@ -1480,30 +2373,33 @@
         <v>3</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="K26" s="1">
         <v>18.964343237000001</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L26" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C27" t="s">
         <v>5</v>
@@ -1512,33 +2408,36 @@
         <v>3</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="K27" s="1">
         <v>18.986342571000002</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L27" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C28" t="s">
         <v>2</v>
@@ -1547,33 +2446,36 @@
         <v>3</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="K28" s="1">
         <v>11.325136212</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L28" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C29" t="s">
         <v>2</v>
@@ -1582,36 +2484,39 @@
         <v>3</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="K29" s="1">
         <v>40.484891871999999</v>
       </c>
-      <c r="L29" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L29" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="M29" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C30" t="s">
         <v>2</v>
@@ -1620,33 +2525,36 @@
         <v>3</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="K30" s="1">
         <v>38.229036952000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L30" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C31" t="s">
         <v>2</v>
@@ -1654,34 +2562,34 @@
       <c r="D31" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="4" t="s">
-        <v>59</v>
+      <c r="E31" s="14" t="s">
+        <v>93</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="K31" s="1">
         <v>32.788524181</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C32" t="s">
         <v>2</v>
@@ -1689,34 +2597,34 @@
       <c r="D32" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="4" t="s">
-        <v>59</v>
+      <c r="E32" s="14" t="s">
+        <v>93</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="K32" s="1">
         <v>32.759743379</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C33" t="s">
         <v>2</v>
@@ -1725,33 +2633,36 @@
         <v>3</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="K33" s="1">
         <v>8.2013932080000007</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L33" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C34" t="s">
         <v>2</v>
@@ -1760,33 +2671,36 @@
         <v>3</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="K34" s="1">
         <v>40.388901236000002</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L34" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
@@ -1795,33 +2709,36 @@
         <v>6</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="K35" s="1">
         <v>19.008362587000001</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L35" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C36" t="s">
         <v>2</v>
@@ -1829,28 +2746,31 @@
       <c r="D36" t="s">
         <v>7</v>
       </c>
-      <c r="E36" s="4" t="s">
-        <v>58</v>
+      <c r="E36" s="14" t="s">
+        <v>95</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H36" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="J36" s="4" t="s">
-        <v>58</v>
+      <c r="H36" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="J36" s="14" t="s">
+        <v>95</v>
       </c>
       <c r="K36" s="1">
         <v>38.472231819000001</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L36" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C37" t="s">
         <v>2</v>
@@ -1859,33 +2779,36 @@
         <v>7</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>58</v>
+        <v>96</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>58</v>
+        <v>96</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="K37" s="1">
         <v>38.425875333</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L37" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C38" t="s">
         <v>2</v>
@@ -1894,32 +2817,323 @@
         <v>3</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="K38" s="1">
         <v>16.553534907</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B40" s="6" t="s">
+      <c r="L38" s="7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>63</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="I39" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="J39" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="K39" s="1">
+        <v>40.799999999999997</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>68</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="I40" s="6"/>
+      <c r="J40" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="K40" s="1">
+        <v>115.73568678399999</v>
+      </c>
+      <c r="M40" s="13"/>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41">
+        <v>40</v>
+      </c>
       <c r="B41" t="s">
-        <v>20</v>
+        <v>59</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I41" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="J41" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="M41" s="13"/>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>60</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H42" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I42" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="J42" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="M42" s="13"/>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>72</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="H44" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="I44" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="J44" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>73</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="H45" s="6"/>
+      <c r="I45" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J45" s="6"/>
+      <c r="K45" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>74</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="H46" s="6"/>
+      <c r="I46" s="6"/>
+      <c r="J46" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="K46" s="1">
+        <v>90.2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>75</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="H47" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I47" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J47" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="K47" s="1">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>77</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F48" s="6"/>
+      <c r="G48" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="H48" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="I48" s="6"/>
+      <c r="J48" s="16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>78</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="H49" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="I49" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="J49" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="B51" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G51" s="4"/>
+      <c r="H51" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="B52" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="B53" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="B54" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>